<commit_message>
Feat: testes modelos + resultados
</commit_message>
<xml_diff>
--- a/outputs/mamografia/Resultados Detecção.xlsx
+++ b/outputs/mamografia/Resultados Detecção.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d44dd37942931253/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\PythonNotebooks\Radiomica\outputs\mamografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="8_{BA9D5DEA-9DD2-48D6-9C5F-C47B76753328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95749FFF-27E1-4941-8701-448ACCD72B61}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641FE456-91E0-4B05-9F3A-F4E75031F955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{1232911C-D2E0-44C2-B4F6-C48FDF41E84E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="2" xr2:uid="{1232911C-D2E0-44C2-B4F6-C48FDF41E84E}"/>
   </bookViews>
   <sheets>
     <sheet name="MIAS" sheetId="1" r:id="rId1"/>
+    <sheet name="INBREAST" sheetId="2" r:id="rId2"/>
+    <sheet name="CBIS-DDSM" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="18">
   <si>
     <t>Tipo de imagem</t>
   </si>
@@ -94,7 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +106,21 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -213,10 +230,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -233,7 +251,32 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -245,30 +288,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -582,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{232BBAC7-42DC-4DC9-9619-F466167F625F}">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +631,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -609,7 +641,7 @@
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -624,7 +656,7 @@
       <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="3" t="s">
@@ -632,34 +664,34 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="19" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="7">
         <v>0.56097560999999996</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="19" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="7">
         <v>0.6504065</v>
       </c>
       <c r="M2" s="1"/>
@@ -667,22 +699,22 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="12"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="20"/>
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="8">
         <v>0.45528455000000001</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="12"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="20"/>
       <c r="J3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="8">
         <v>0.65040651000000005</v>
       </c>
       <c r="M3" s="1"/>
@@ -690,22 +722,22 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="12"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="8">
         <v>0.43902438999999999</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="12"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="20"/>
       <c r="J4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="8">
         <v>0.66666667000000002</v>
       </c>
       <c r="M4" s="1"/>
@@ -713,22 +745,22 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="12"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="8">
         <v>0.57723577000000004</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="12"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="20"/>
       <c r="J5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="8">
         <v>0.56910569</v>
       </c>
       <c r="M5" s="1"/>
@@ -736,22 +768,22 @@
       <c r="O5" s="1"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="12"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="8">
         <v>0.46341462999999999</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="12"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="20"/>
       <c r="J6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="8">
         <v>0.70731706999999999</v>
       </c>
       <c r="M6" s="1"/>
@@ -759,22 +791,22 @@
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="12"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="8">
         <v>0.57723577000000004</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="12"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="20"/>
       <c r="J7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="8">
         <v>0.60162601999999998</v>
       </c>
       <c r="M7" s="1"/>
@@ -782,23 +814,23 @@
       <c r="O7" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="5">
         <v>0.42276423000000002</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="7" t="s">
+      <c r="G8" s="17"/>
+      <c r="H8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="10" t="s">
+      <c r="I8" s="17"/>
+      <c r="J8" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K8" s="5">
@@ -809,18 +841,18 @@
       <c r="O8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="5">
         <v>0.48780488</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
       <c r="J9" s="4" t="s">
         <v>10</v>
       </c>
@@ -832,9 +864,9 @@
       <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -842,9 +874,9 @@
         <v>0.45528455000000001</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
       <c r="J10" s="4" t="s">
         <v>11</v>
       </c>
@@ -857,9 +889,9 @@
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -867,9 +899,9 @@
         <v>0.55284553000000003</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
       <c r="J11" s="4" t="s">
         <v>12</v>
       </c>
@@ -882,9 +914,9 @@
       <c r="O11" s="1"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -892,9 +924,9 @@
         <v>0.46341463999999999</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
       <c r="J12" s="4" t="s">
         <v>13</v>
       </c>
@@ -907,9 +939,9 @@
       <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="8"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -917,9 +949,9 @@
         <v>0.51219512</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="8"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="17"/>
       <c r="J13" s="4" t="s">
         <v>14</v>
       </c>
@@ -932,11 +964,11 @@
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="17"/>
+      <c r="B14" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="8"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
@@ -944,11 +976,11 @@
         <v>0.54471544999999999</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="6" t="s">
+      <c r="G14" s="17"/>
+      <c r="H14" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="8"/>
+      <c r="I14" s="17"/>
       <c r="J14" s="4" t="s">
         <v>9</v>
       </c>
@@ -961,9 +993,9 @@
       <c r="O14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="8"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="17"/>
       <c r="D15" s="4" t="s">
         <v>10</v>
       </c>
@@ -971,9 +1003,9 @@
         <v>0.52845527999999997</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="8"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="17"/>
       <c r="J15" s="4" t="s">
         <v>10</v>
       </c>
@@ -986,9 +1018,9 @@
       <c r="O15" s="1"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="8"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="4" t="s">
         <v>11</v>
       </c>
@@ -996,9 +1028,9 @@
         <v>0.60975610000000002</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="8"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="17"/>
       <c r="J16" s="4" t="s">
         <v>11</v>
       </c>
@@ -1011,9 +1043,9 @@
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="8"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="4" t="s">
         <v>12</v>
       </c>
@@ -1021,9 +1053,9 @@
         <v>0.52845527999999997</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="8"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="17"/>
       <c r="J17" s="4" t="s">
         <v>12</v>
       </c>
@@ -1036,9 +1068,9 @@
       <c r="O17" s="1"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="8"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1046,9 +1078,9 @@
         <v>0.41463414999999998</v>
       </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="8"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="17"/>
       <c r="J18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1061,9 +1093,9 @@
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="9"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="18"/>
       <c r="D19" s="4" t="s">
         <v>14</v>
       </c>
@@ -1071,9 +1103,9 @@
         <v>0.55284553000000003</v>
       </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="9"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="18"/>
       <c r="J19" s="4" t="s">
         <v>14</v>
       </c>
@@ -1086,31 +1118,31 @@
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="7" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="7">
         <v>0.60975610000000002</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="7" t="s">
+      <c r="G20" s="17"/>
+      <c r="H20" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="19" t="s">
         <v>17</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K20" s="13">
+      <c r="K20" s="7">
         <v>0.63414634000000003</v>
       </c>
       <c r="L20" s="1"/>
@@ -1119,23 +1151,23 @@
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="12"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="8">
         <v>0.55284553000000003</v>
       </c>
       <c r="F21" s="1"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="12"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="20"/>
       <c r="J21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K21" s="14">
+      <c r="K21" s="8">
         <v>0.68292682999999998</v>
       </c>
       <c r="L21" s="1"/>
@@ -1144,23 +1176,23 @@
       <c r="O21" s="1"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="12"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="8">
         <v>0.42276423000000002</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="12"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="20"/>
       <c r="J22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K22" s="14">
+      <c r="K22" s="8">
         <v>0.70731706999999999</v>
       </c>
       <c r="L22" s="1"/>
@@ -1169,23 +1201,23 @@
       <c r="O22" s="1"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="12"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="8">
         <v>0.51219512</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="12"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="20"/>
       <c r="J23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K23" s="14">
+      <c r="K23" s="8">
         <v>0.68292682999999998</v>
       </c>
       <c r="L23" s="1"/>
@@ -1194,23 +1226,23 @@
       <c r="O23" s="1"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="12"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="8">
         <v>0.45528455000000001</v>
       </c>
       <c r="F24" s="1"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="12"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="20"/>
       <c r="J24" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K24" s="14">
+      <c r="K24" s="8">
         <v>0.69918698999999995</v>
       </c>
       <c r="L24" s="1"/>
@@ -1219,23 +1251,23 @@
       <c r="O24" s="1"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="12"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="8">
         <v>0.58536586000000002</v>
       </c>
       <c r="F25" s="1"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="12"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="20"/>
       <c r="J25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="14">
+      <c r="K25" s="8">
         <v>0.68292682999999998</v>
       </c>
       <c r="L25" s="1"/>
@@ -1244,24 +1276,24 @@
       <c r="O25" s="1"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="7" t="s">
+      <c r="A26" s="17"/>
+      <c r="B26" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="10" t="s">
+      <c r="C26" s="17"/>
+      <c r="D26" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="5">
         <v>0.50406503999999996</v>
       </c>
       <c r="F26" s="1"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="7" t="s">
+      <c r="G26" s="17"/>
+      <c r="H26" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="8"/>
-      <c r="J26" s="10" t="s">
+      <c r="I26" s="17"/>
+      <c r="J26" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K26" s="5">
@@ -1273,18 +1305,18 @@
       <c r="O26" s="1"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
       <c r="D27" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="5">
         <v>0.58536584999999997</v>
       </c>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
       <c r="J27" s="4" t="s">
         <v>10</v>
       </c>
@@ -1293,18 +1325,18 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
       <c r="D28" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="5">
         <v>0.56097560999999996</v>
       </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
       <c r="J28" s="4" t="s">
         <v>11</v>
       </c>
@@ -1313,18 +1345,18 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
       <c r="D29" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E29" s="5">
         <v>0.56097560999999996</v>
       </c>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
       <c r="J29" s="4" t="s">
         <v>12</v>
       </c>
@@ -1333,38 +1365,38 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="16">
+      <c r="E30" s="10">
         <v>0.45528455000000001</v>
       </c>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
       <c r="J30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K30" s="16">
+      <c r="K30" s="10">
         <v>0.6504065</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="8"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="17"/>
       <c r="D31" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E31" s="5">
         <v>0.57723577000000004</v>
       </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="8"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="17"/>
       <c r="J31" s="4" t="s">
         <v>14</v>
       </c>
@@ -1373,22 +1405,22 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="6" t="s">
+      <c r="A32" s="17"/>
+      <c r="B32" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="8"/>
+      <c r="C32" s="17"/>
       <c r="D32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E32" s="5">
         <v>0.52845529000000002</v>
       </c>
-      <c r="G32" s="8"/>
-      <c r="H32" s="6" t="s">
+      <c r="G32" s="17"/>
+      <c r="H32" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I32" s="8"/>
+      <c r="I32" s="17"/>
       <c r="J32" s="4" t="s">
         <v>9</v>
       </c>
@@ -1397,18 +1429,18 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="8"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="17"/>
       <c r="D33" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E33" s="5">
         <v>0.55284553000000003</v>
       </c>
-      <c r="G33" s="8"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="8"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="17"/>
       <c r="J33" s="4" t="s">
         <v>10</v>
       </c>
@@ -1417,18 +1449,18 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="8"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="5">
         <v>0.56910569</v>
       </c>
-      <c r="G34" s="8"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="8"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="17"/>
       <c r="J34" s="4" t="s">
         <v>11</v>
       </c>
@@ -1437,18 +1469,18 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="8"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="17"/>
       <c r="D35" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E35" s="5">
         <v>0.62601625999999999</v>
       </c>
-      <c r="G35" s="8"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="8"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="17"/>
       <c r="J35" s="4" t="s">
         <v>12</v>
       </c>
@@ -1457,18 +1489,18 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="8"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="17"/>
       <c r="D36" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E36" s="5">
         <v>0.50406503999999996</v>
       </c>
-      <c r="G36" s="8"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="8"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="17"/>
       <c r="J36" s="4" t="s">
         <v>13</v>
       </c>
@@ -1477,18 +1509,18 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="9"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="18"/>
       <c r="D37" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E37" s="5">
         <v>0.54471544999999999</v>
       </c>
-      <c r="G37" s="9"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="9"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="18"/>
       <c r="J37" s="4" t="s">
         <v>14</v>
       </c>
@@ -1520,4 +1552,1724 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC5D124-4E49-4D63-818B-BC0CB96BABD0}">
+  <dimension ref="A1:L37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="12">
+        <v>0.58700209999999997</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="7">
+        <v>0.84905660999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="13">
+        <v>0.60587002000000001</v>
+      </c>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0.83857442000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0.47589098000000002</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0.81551362999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.57651991999999996</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0.85324946999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.52410902000000004</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0.83647799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.48637317000000002</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0.86792453000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0.66666667000000002</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0.49637316999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.63522012999999999</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0.89308175999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0.59538784</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0.87631026999999995</v>
+      </c>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="11">
+        <v>0.65828092000000005</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0.88679244999999995</v>
+      </c>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0.59119496999999999</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0.87211740000000004</v>
+      </c>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0.52201257999999995</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0.88050313999999996</v>
+      </c>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+      <c r="B14" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="11">
+        <v>0.58490565999999999</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="17"/>
+      <c r="J14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14" s="11">
+        <v>0.57442347999999999</v>
+      </c>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0.55345911999999997</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="11">
+        <v>0.89937107000000005</v>
+      </c>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0.57651991999999996</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0.87421384000000002</v>
+      </c>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0.56603773999999996</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0.89727462999999996</v>
+      </c>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="11">
+        <v>0.53878406999999995</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="11">
+        <v>0.88259958000000005</v>
+      </c>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="11">
+        <v>0.54926624999999996</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="11">
+        <v>0.88679244999999995</v>
+      </c>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="B20" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="12">
+        <v>0.66666667000000002</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="7">
+        <v>0.85115304000000003</v>
+      </c>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0.59329140000000002</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="8">
+        <v>0.82809224999999997</v>
+      </c>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="13">
+        <v>0.48637317000000002</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="13">
+        <v>0.82809224000000003</v>
+      </c>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0.60796645999999999</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="8">
+        <v>0.8427673</v>
+      </c>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="13">
+        <v>0.51362684000000003</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K24" s="8">
+        <v>0.83857442000000004</v>
+      </c>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="13">
+        <v>0.56813416999999999</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K25" s="8">
+        <v>0.84696017000000001</v>
+      </c>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="17"/>
+      <c r="B26" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="11">
+        <v>0.68343816000000002</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="17"/>
+      <c r="J26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K26" s="5">
+        <v>0.53249475999999996</v>
+      </c>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="11">
+        <v>0.68972745999999996</v>
+      </c>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K27" s="5">
+        <v>0.87631026999999995</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="11">
+        <v>0.58071278999999998</v>
+      </c>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="5">
+        <v>0.85744235000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="11">
+        <v>0.70020963999999997</v>
+      </c>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K29" s="5">
+        <v>0.87421384000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="15">
+        <v>0.64360587000000002</v>
+      </c>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30" s="10">
+        <v>0.86792453000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="11">
+        <v>0.66666667000000002</v>
+      </c>
+      <c r="G31" s="17"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K31" s="5">
+        <v>0.88888889000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="17"/>
+      <c r="B32" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="11">
+        <v>0.67505241000000005</v>
+      </c>
+      <c r="G32" s="17"/>
+      <c r="H32" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="17"/>
+      <c r="J32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" s="5">
+        <v>0.53459118999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="11">
+        <v>0.69811321000000004</v>
+      </c>
+      <c r="G33" s="17"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K33" s="5">
+        <v>0.90775680999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="17"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="11">
+        <v>0.62683438000000002</v>
+      </c>
+      <c r="G34" s="17"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K34" s="5">
+        <v>0.87421384000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="11">
+        <v>0.69182390000000005</v>
+      </c>
+      <c r="F35" s="14"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" s="5">
+        <v>0.89517818999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="11">
+        <v>0.66247378999999995</v>
+      </c>
+      <c r="G36" s="17"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" s="5">
+        <v>0.89308175999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="11">
+        <v>0.66247378999999995</v>
+      </c>
+      <c r="G37" s="18"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K37" s="5">
+        <v>0.89517820000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="I2:I19"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="H8:H13"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="H14:H19"/>
+    <mergeCell ref="A2:A37"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="C2:C19"/>
+    <mergeCell ref="G2:G37"/>
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="C20:C37"/>
+    <mergeCell ref="H20:H25"/>
+    <mergeCell ref="I20:I37"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="H26:H31"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="H32:H37"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDCD4671-BAB5-4FFF-9AB8-E77302E070D5}">
+  <dimension ref="A1:K37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="12">
+        <v>0.56004619</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="7">
+        <v>0.53153152999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="13">
+        <v>0.54849884999999998</v>
+      </c>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0.55092048999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0.53887605999999999</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0.54524088999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.54580446999999999</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0.55248726999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.54234026000000002</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0.55816686000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.53656658999999995</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0.54191148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0.49653578999999998</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0.56619662999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.57351808999999998</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0.58969839000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0.55080830999999997</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0.54034468999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="11">
+        <v>0.56735950999999996</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0.58617313000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0.58275597000000001</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0.59322366000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0.56966897999999999</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0.53701527999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+      <c r="B14" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="11">
+        <v>0.49961508999999998</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="17"/>
+      <c r="J14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14" s="11">
+        <v>0.54308656</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0.58737490000000003</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="11">
+        <v>0.59596552999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0.59738259999999999</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0.54151978000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0.57659738000000005</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0.58754406999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="11">
+        <v>0.57505773999999998</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="11">
+        <v>0.58852329999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="11">
+        <v>0.58121632000000001</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="11">
+        <v>0.54171563</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="B20" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="12">
+        <v>0.57351808999999998</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="7">
+        <v>0.52017234999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0.56812932999999999</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="8">
+        <v>0.54896199999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="13">
+        <v>0.55658198999999997</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="13">
+        <v>0.54857031000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0.56697458999999995</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="8">
+        <v>0.54876616</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="13">
+        <v>0.55542725000000004</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K24" s="8">
+        <v>0.56090874000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="13">
+        <v>0.56158584</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K25" s="8">
+        <v>0.55483744999999995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="17"/>
+      <c r="B26" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="11">
+        <v>0.49345651000000001</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="17"/>
+      <c r="J26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K26" s="5">
+        <v>0.55992949000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="11">
+        <v>0.58699000000000001</v>
+      </c>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K27" s="5">
+        <v>0.58813161000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="11">
+        <v>0.61431871000000005</v>
+      </c>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="5">
+        <v>0.55307481000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="11">
+        <v>0.57043880000000002</v>
+      </c>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K29" s="5">
+        <v>0.57853505999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="15">
+        <v>0.57698229000000001</v>
+      </c>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30" s="10">
+        <v>0.58519388999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="11">
+        <v>0.58314087999999997</v>
+      </c>
+      <c r="G31" s="17"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K31" s="5">
+        <v>0.51331766999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="17"/>
+      <c r="B32" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="11">
+        <v>0.50885296000000002</v>
+      </c>
+      <c r="G32" s="17"/>
+      <c r="H32" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="17"/>
+      <c r="J32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" s="5">
+        <v>0.53584019000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="11">
+        <v>0.59584294999999998</v>
+      </c>
+      <c r="G33" s="17"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K33" s="5">
+        <v>0.57363885999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="17"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="11">
+        <v>0.58237105</v>
+      </c>
+      <c r="G34" s="17"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K34" s="5">
+        <v>0.55660008000000005</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="11">
+        <v>0.60161662999999999</v>
+      </c>
+      <c r="F35" s="14"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" s="5">
+        <v>0.57363885000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="11">
+        <v>0.58698998999999996</v>
+      </c>
+      <c r="G36" s="17"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" s="5">
+        <v>0.58088523000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="11">
+        <v>0.56966897999999999</v>
+      </c>
+      <c r="G37" s="18"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K37" s="5">
+        <v>0.55268311999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="I2:I19"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="H8:H13"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="H14:H19"/>
+    <mergeCell ref="A2:A37"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="C2:C19"/>
+    <mergeCell ref="G2:G37"/>
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="C20:C37"/>
+    <mergeCell ref="H20:H25"/>
+    <mergeCell ref="I20:I37"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="H26:H31"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="H32:H37"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>